<commit_message>
Corrected Nov 22 data
FlHealthCHARTS was a late update.
</commit_message>
<xml_diff>
--- a/113 other and unspecified_COVID/RES 113 other and unspecified race 2020Nov22.xlsx
+++ b/113 other and unspecified_COVID/RES 113 other and unspecified race 2020Nov22.xlsx
@@ -83,832 +83,832 @@
     <t>4</t>
   </si>
   <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Baker</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Bay</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Brevard</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>317</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>388</t>
+  </si>
+  <si>
+    <t>377</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>455</t>
+  </si>
+  <si>
+    <t>Broward</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>906</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>1,501</t>
+  </si>
+  <si>
+    <t>1,024</t>
+  </si>
+  <si>
+    <t>554</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>1,661</t>
+  </si>
+  <si>
+    <t>Calhoun</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>Citrus</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Collier</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>283</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>Miami-Dade</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>2,470</t>
+  </si>
+  <si>
+    <t>552</t>
+  </si>
+  <si>
+    <t>3,102</t>
+  </si>
+  <si>
+    <t>2,648</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>3,332</t>
+  </si>
+  <si>
+    <t>Desoto</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Dixie</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Duval</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>547</t>
+  </si>
+  <si>
+    <t>372</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>649</t>
+  </si>
+  <si>
+    <t>Escambia</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>251</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>Flagler</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Gadsden</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Gilchrist</t>
+  </si>
+  <si>
+    <t>Glades</t>
+  </si>
+  <si>
+    <t>Gulf</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Hardee</t>
+  </si>
+  <si>
+    <t>Hendry</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Hernando</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>Highlands</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>Hillsborough</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>595</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>768</t>
+  </si>
+  <si>
+    <t>698</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>897</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>Indian River</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Lafayette</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>436</t>
+  </si>
+  <si>
+    <t>489</t>
+  </si>
+  <si>
+    <t>509</t>
+  </si>
+  <si>
+    <t>571</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Levy</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Manatee</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>323</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
     <t>49</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>89</t>
+    <t>312</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>Nassau</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>Okaloosa</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>Okeechobee</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>379</t>
+  </si>
+  <si>
+    <t>599</t>
+  </si>
+  <si>
+    <t>481</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>738</t>
+  </si>
+  <si>
+    <t>Osceola</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>Palm Beach</t>
+  </si>
+  <si>
+    <t>1,006</t>
+  </si>
+  <si>
+    <t>1,319</t>
+  </si>
+  <si>
+    <t>1,132</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>1,470</t>
+  </si>
+  <si>
+    <t>Pasco</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
+  <si>
+    <t>Pinellas</t>
+  </si>
+  <si>
+    <t>479</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>594</t>
+  </si>
+  <si>
+    <t>615</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>742</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>591</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
+    <t>Putnam</t>
+  </si>
+  <si>
+    <t>Saint Johns</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Saint Lucie</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>314</t>
+  </si>
+  <si>
+    <t>263</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>Santa Rosa</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Sarasota</t>
+  </si>
+  <si>
+    <t>295</t>
+  </si>
+  <si>
+    <t>Seminole</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>Sumter</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>Suwannee</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Union</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>Baker</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Bay</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>Bradford</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Brevard</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>309</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>379</t>
-  </si>
-  <si>
-    <t>369</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>446</t>
-  </si>
-  <si>
-    <t>Broward</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>883</t>
+    <t>Volusia</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>327</t>
+  </si>
+  <si>
+    <t>343</t>
+  </si>
+  <si>
+    <t>406</t>
+  </si>
+  <si>
+    <t>Wakulla</t>
+  </si>
+  <si>
+    <t>Walton</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>438</t>
+  </si>
+  <si>
+    <t>368</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>434</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>466</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>478</t>
+  </si>
+  <si>
+    <t>11,751</t>
+  </si>
+  <si>
+    <t>3,051</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>15,283</t>
+  </si>
+  <si>
+    <t>13,635</t>
+  </si>
+  <si>
+    <t>3,352</t>
   </si>
   <si>
     <t>518</t>
   </si>
   <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>1,475</t>
-  </si>
-  <si>
-    <t>1,001</t>
-  </si>
-  <si>
-    <t>552</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>1,635</t>
-  </si>
-  <si>
-    <t>Calhoun</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>188</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
-    <t>Citrus</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Clay</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>Collier</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>277</t>
-  </si>
-  <si>
-    <t>Columbia</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>Miami-Dade</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>2,448</t>
-  </si>
-  <si>
-    <t>548</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>3,076</t>
-  </si>
-  <si>
-    <t>2,626</t>
-  </si>
-  <si>
-    <t>596</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>3,306</t>
-  </si>
-  <si>
-    <t>Desoto</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Dixie</t>
-  </si>
-  <si>
-    <t>Duval</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>299</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>535</t>
-  </si>
-  <si>
-    <t>365</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>637</t>
-  </si>
-  <si>
-    <t>Escambia</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>248</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>279</t>
-  </si>
-  <si>
-    <t>Flagler</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Franklin</t>
-  </si>
-  <si>
-    <t>Gadsden</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>Gilchrist</t>
-  </si>
-  <si>
-    <t>Glades</t>
-  </si>
-  <si>
-    <t>Gulf</t>
-  </si>
-  <si>
-    <t>Hamilton</t>
-  </si>
-  <si>
-    <t>Hardee</t>
-  </si>
-  <si>
-    <t>Hendry</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Hernando</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>163</t>
-  </si>
-  <si>
-    <t>Highlands</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Hillsborough</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>578</t>
-  </si>
-  <si>
-    <t>747</t>
-  </si>
-  <si>
-    <t>681</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>876</t>
-  </si>
-  <si>
-    <t>Holmes</t>
-  </si>
-  <si>
-    <t>Indian River</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>Jefferson</t>
-  </si>
-  <si>
-    <t>Lafayette</t>
-  </si>
-  <si>
-    <t>Lake</t>
-  </si>
-  <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>215</t>
-  </si>
-  <si>
-    <t>213</t>
-  </si>
-  <si>
-    <t>258</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>480</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>562</t>
-  </si>
-  <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>Levy</t>
-  </si>
-  <si>
-    <t>Liberty</t>
-  </si>
-  <si>
-    <t>Madison</t>
-  </si>
-  <si>
-    <t>Manatee</t>
-  </si>
-  <si>
-    <t>260</t>
-  </si>
-  <si>
-    <t>315</t>
-  </si>
-  <si>
-    <t>293</t>
-  </si>
-  <si>
-    <t>351</t>
-  </si>
-  <si>
-    <t>Marion</t>
-  </si>
-  <si>
-    <t>252</t>
-  </si>
-  <si>
-    <t>307</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>358</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>162</t>
-  </si>
-  <si>
-    <t>Monroe</t>
-  </si>
-  <si>
-    <t>Nassau</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>Okaloosa</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>Okeechobee</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>370</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>587</t>
-  </si>
-  <si>
-    <t>472</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>726</t>
-  </si>
-  <si>
-    <t>Osceola</t>
-  </si>
-  <si>
-    <t>181</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>Palm Beach</t>
-  </si>
-  <si>
-    <t>992</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
-    <t>1,302</t>
-  </si>
-  <si>
-    <t>1,118</t>
-  </si>
-  <si>
-    <t>302</t>
-  </si>
-  <si>
-    <t>1,453</t>
-  </si>
-  <si>
-    <t>Pasco</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>214</t>
-  </si>
-  <si>
-    <t>249</t>
-  </si>
-  <si>
-    <t>266</t>
-  </si>
-  <si>
-    <t>Pinellas</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>585</t>
-  </si>
-  <si>
-    <t>608</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>733</t>
-  </si>
-  <si>
-    <t>Polk</t>
-  </si>
-  <si>
-    <t>439</t>
-  </si>
-  <si>
-    <t>579</t>
-  </si>
-  <si>
-    <t>509</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>665</t>
-  </si>
-  <si>
-    <t>Putnam</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>Saint Johns</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>Saint Lucie</t>
-  </si>
-  <si>
-    <t>229</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>305</t>
-  </si>
-  <si>
-    <t>256</t>
-  </si>
-  <si>
-    <t>339</t>
-  </si>
-  <si>
-    <t>Santa Rosa</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Sarasota</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>251</t>
-  </si>
-  <si>
-    <t>283</t>
-  </si>
-  <si>
-    <t>311</t>
-  </si>
-  <si>
-    <t>Seminole</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>255</t>
-  </si>
-  <si>
-    <t>Sumter</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>Suwannee</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Union</t>
-  </si>
-  <si>
-    <t>Volusia</t>
-  </si>
-  <si>
-    <t>319</t>
-  </si>
-  <si>
-    <t>335</t>
-  </si>
-  <si>
-    <t>398</t>
-  </si>
-  <si>
-    <t>Wakulla</t>
-  </si>
-  <si>
-    <t>Walton</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>357</t>
-  </si>
-  <si>
-    <t>417</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>438</t>
-  </si>
-  <si>
-    <t>368</t>
-  </si>
-  <si>
-    <t>434</t>
-  </si>
-  <si>
-    <t>466</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>478</t>
-  </si>
-  <si>
-    <t>11,491</t>
-  </si>
-  <si>
-    <t>3,015</t>
-  </si>
-  <si>
-    <t>14,982</t>
-  </si>
-  <si>
-    <t>13,375</t>
-  </si>
-  <si>
-    <t>3,316</t>
-  </si>
-  <si>
-    <t>513</t>
-  </si>
-  <si>
-    <t>17,215</t>
+    <t>17,516</t>
   </si>
   <si>
     <t>Resident Deaths by Residence County by Year by Race
@@ -1855,16 +1855,16 @@
         <v>53</v>
       </c>
       <c r="AD10" s="20" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="14.65">
       <c r="A11" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>30</v>
@@ -1876,7 +1876,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>30</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>43</v>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="M11" s="19"/>
       <c r="N11" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O11" s="19" t="s">
         <v>29</v>
@@ -1911,48 +1911,48 @@
         <v>20</v>
       </c>
       <c r="R11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="T11" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="T11" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="U11" s="19"/>
       <c r="V11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="W11" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="W11" s="19" t="s">
+      <c r="X11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="X11" s="19" t="s">
+      <c r="Y11" s="19" t="s">
         <v>64</v>
-      </c>
-      <c r="Y11" s="19" t="s">
-        <v>65</v>
       </c>
       <c r="Z11" s="19"/>
       <c r="AA11" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB11" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AB11" s="20" t="s">
+      <c r="AC11" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="AC11" s="20" t="s">
+      <c r="AD11" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="AD11" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="AE11" s="20"/>
       <c r="AF11" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="14.65">
       <c r="A12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -1990,10 +1990,10 @@
       </c>
       <c r="Z12" s="19"/>
       <c r="AA12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB12" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="AB12" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="AC12" s="20" t="s">
         <v>15</v>
@@ -2003,12 +2003,12 @@
       </c>
       <c r="AE12" s="20"/>
       <c r="AF12" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="14.65">
       <c r="A13" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>41</v>
@@ -2036,7 +2036,7 @@
         <v>19</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>15</v>
@@ -2054,35 +2054,35 @@
         <v>17</v>
       </c>
       <c r="W13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X13" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y13" s="19" t="s">
         <v>15</v>
       </c>
       <c r="Z13" s="19"/>
       <c r="AA13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB13" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AB13" s="20" t="s">
-        <v>75</v>
-      </c>
       <c r="AC13" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD13" s="20" t="s">
         <v>15</v>
       </c>
       <c r="AE13" s="20"/>
       <c r="AF13" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="14.65">
       <c r="A14" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>20</v>
@@ -2126,7 +2126,7 @@
         <v>21</v>
       </c>
       <c r="W14" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X14" s="19" t="s">
         <v>19</v>
@@ -2134,10 +2134,10 @@
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
       <c r="AA14" s="20" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="AB14" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AC14" s="20" t="s">
         <v>19</v>
@@ -2145,12 +2145,12 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
       <c r="AF14" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="14.65">
       <c r="A15" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>16</v>
@@ -2197,38 +2197,38 @@
       </c>
       <c r="U15" s="19"/>
       <c r="V15" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W15" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X15" s="19" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="Y15" s="19" t="s">
         <v>17</v>
       </c>
       <c r="Z15" s="19"/>
       <c r="AA15" s="20" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="AB15" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC15" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE15" s="20"/>
       <c r="AF15" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="14.65">
       <c r="A16" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>19</v>
@@ -2257,15 +2257,15 @@
         <v>15</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O16" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
       <c r="R16" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S16" s="19" t="s">
         <v>40</v>
@@ -2276,7 +2276,7 @@
         <v>40</v>
       </c>
       <c r="W16" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X16" s="19" t="s">
         <v>46</v>
@@ -2286,10 +2286,10 @@
       </c>
       <c r="Z16" s="19"/>
       <c r="AA16" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB16" s="20" t="s">
         <v>89</v>
-      </c>
-      <c r="AB16" s="20" t="s">
-        <v>90</v>
       </c>
       <c r="AC16" s="20" t="s">
         <v>43</v>
@@ -2299,12 +2299,12 @@
       </c>
       <c r="AE16" s="20"/>
       <c r="AF16" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="14.65">
       <c r="A17" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -2348,23 +2348,23 @@
         <v>16</v>
       </c>
       <c r="W17" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X17" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Y17" s="19" t="s">
         <v>20</v>
       </c>
       <c r="Z17" s="19"/>
       <c r="AA17" s="20" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="AB17" s="20" t="s">
         <v>94</v>
       </c>
       <c r="AC17" s="20" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="AD17" s="20" t="s">
         <v>20</v>
@@ -2394,7 +2394,7 @@
         <v>99</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -2402,14 +2402,14 @@
         <v>100</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>31</v>
@@ -2419,54 +2419,54 @@
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S18" s="19" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="T18" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U18" s="19" t="s">
         <v>15</v>
       </c>
       <c r="V18" s="20" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="W18" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="X18" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Y18" s="19" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="Z18" s="19" t="s">
         <v>19</v>
       </c>
       <c r="AA18" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AB18" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC18" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AD18" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AE18" s="20" t="s">
         <v>19</v>
       </c>
       <c r="AF18" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="14.65">
       <c r="A19" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -2502,7 +2502,7 @@
         <v>15</v>
       </c>
       <c r="W19" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X19" s="19" t="s">
         <v>19</v>
@@ -2510,10 +2510,10 @@
       <c r="Y19" s="19"/>
       <c r="Z19" s="19"/>
       <c r="AA19" s="20" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="AB19" s="20" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="AC19" s="20" t="s">
         <v>17</v>
@@ -2521,12 +2521,12 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
       <c r="AF19" s="20" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="14.65">
       <c r="A20" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>15</v>
@@ -2570,10 +2570,10 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
       <c r="AA20" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB20" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="AB20" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="AC20" s="20" t="s">
         <v>20</v>
@@ -2586,10 +2586,10 @@
     </row>
     <row r="21" spans="1:32" ht="14.65">
       <c r="A21" s="18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>17</v>
@@ -2612,17 +2612,17 @@
         <v>47</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="O21" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="P21" s="19" t="s">
         <v>19</v>
@@ -2631,7 +2631,7 @@
         <v>15</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="S21" s="19" t="s">
         <v>46</v>
@@ -2646,35 +2646,35 @@
         <v>30</v>
       </c>
       <c r="W21" s="19" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="X21" s="19" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="Y21" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z21" s="19"/>
       <c r="AA21" s="20" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AB21" s="20" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AC21" s="20" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AD21" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AE21" s="20"/>
       <c r="AF21" s="20" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="14.65">
       <c r="A22" s="18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>20</v>
@@ -2695,7 +2695,7 @@
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>19</v>
@@ -2730,35 +2730,35 @@
         <v>21</v>
       </c>
       <c r="W22" s="19" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="X22" s="19" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="Y22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Z22" s="19"/>
       <c r="AA22" s="20" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AB22" s="20" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AC22" s="20" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="AD22" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE22" s="20"/>
       <c r="AF22" s="20" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="14.65">
       <c r="A23" s="18" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>15</v>
@@ -2800,7 +2800,7 @@
         <v>21</v>
       </c>
       <c r="W23" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X23" s="19" t="s">
         <v>21</v>
@@ -2810,10 +2810,10 @@
       </c>
       <c r="Z23" s="19"/>
       <c r="AA23" s="20" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="AB23" s="20" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="AC23" s="20" t="s">
         <v>21</v>
@@ -2823,12 +2823,12 @@
       </c>
       <c r="AE23" s="20"/>
       <c r="AF23" s="20" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="14.65">
       <c r="A24" s="18" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>15</v>
@@ -2883,12 +2883,12 @@
       <c r="AD24" s="20"/>
       <c r="AE24" s="20"/>
       <c r="AF24" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="14.65">
       <c r="A25" s="18" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19" t="s">
@@ -2933,7 +2933,7 @@
         <v>35</v>
       </c>
       <c r="X25" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
@@ -2941,20 +2941,20 @@
         <v>98</v>
       </c>
       <c r="AB25" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AC25" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
       <c r="AF25" s="20" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="14.65">
       <c r="A26" s="18" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>15</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="27" spans="1:32" ht="14.65">
       <c r="A27" s="18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -3038,35 +3038,35 @@
       <c r="U27" s="19"/>
       <c r="V27" s="20"/>
       <c r="W27" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X27" s="19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="Y27" s="19" t="s">
         <v>15</v>
       </c>
       <c r="Z27" s="19"/>
       <c r="AA27" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AB27" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC27" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AD27" s="20" t="s">
         <v>20</v>
       </c>
       <c r="AE27" s="20"/>
       <c r="AF27" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="14.65">
       <c r="A28" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -3090,7 +3090,7 @@
       <c r="U28" s="19"/>
       <c r="V28" s="20"/>
       <c r="W28" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="X28" s="19" t="s">
         <v>21</v>
@@ -3101,7 +3101,7 @@
         <v>46</v>
       </c>
       <c r="AB28" s="20" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="AC28" s="20" t="s">
         <v>21</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="29" spans="1:32" ht="14.65">
       <c r="A29" s="18" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19" t="s">
@@ -3146,18 +3146,18 @@
       <c r="U29" s="19"/>
       <c r="V29" s="20"/>
       <c r="W29" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="X29" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
       <c r="AA29" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AB29" s="20" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="AC29" s="20" t="s">
         <v>40</v>
@@ -3165,12 +3165,12 @@
       <c r="AD29" s="20"/>
       <c r="AE29" s="20"/>
       <c r="AF29" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="14.65">
       <c r="A30" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -3198,7 +3198,7 @@
       <c r="U30" s="19"/>
       <c r="V30" s="20"/>
       <c r="W30" s="19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="X30" s="19" t="s">
         <v>20</v>
@@ -3206,10 +3206,10 @@
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
       <c r="AA30" s="20" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="AB30" s="20" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="AC30" s="20" t="s">
         <v>20</v>
@@ -3217,12 +3217,12 @@
       <c r="AD30" s="20"/>
       <c r="AE30" s="20"/>
       <c r="AF30" s="20" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="14.65">
       <c r="A31" s="18" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -3258,7 +3258,7 @@
         <v>15</v>
       </c>
       <c r="W31" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X31" s="19" t="s">
         <v>18</v>
@@ -3268,10 +3268,10 @@
       </c>
       <c r="Z31" s="19"/>
       <c r="AA31" s="20" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AB31" s="20" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AC31" s="20" t="s">
         <v>18</v>
@@ -3281,12 +3281,12 @@
       </c>
       <c r="AE31" s="20"/>
       <c r="AF31" s="20" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="14.65">
       <c r="A32" s="18" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>15</v>
@@ -3330,10 +3330,10 @@
         <v>17</v>
       </c>
       <c r="W32" s="19" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="X32" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y32" s="19" t="s">
         <v>16</v>
@@ -3342,13 +3342,13 @@
         <v>15</v>
       </c>
       <c r="AA32" s="20" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AB32" s="20" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AC32" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AD32" s="20" t="s">
         <v>16</v>
@@ -3357,12 +3357,12 @@
         <v>15</v>
       </c>
       <c r="AF32" s="20" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="14.65">
       <c r="A33" s="18" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>20</v>
@@ -3406,35 +3406,35 @@
         <v>19</v>
       </c>
       <c r="W33" s="19" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="X33" s="19" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="Y33" s="19" t="s">
         <v>15</v>
       </c>
       <c r="Z33" s="19"/>
       <c r="AA33" s="20" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="AB33" s="20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AC33" s="20" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="AD33" s="20" t="s">
         <v>15</v>
       </c>
       <c r="AE33" s="20"/>
       <c r="AF33" s="20" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="14.65">
       <c r="A34" s="18" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>31</v>
@@ -3460,7 +3460,7 @@
         <v>32</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L34" s="19" t="s">
         <v>17</v>
@@ -3491,42 +3491,42 @@
         <v>20</v>
       </c>
       <c r="V34" s="20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="W34" s="19" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="X34" s="19" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="Y34" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z34" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA34" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB34" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC34" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD34" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z34" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA34" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB34" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC34" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD34" s="20" t="s">
-        <v>60</v>
-      </c>
       <c r="AE34" s="20" t="s">
         <v>15</v>
       </c>
       <c r="AF34" s="20" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="14.65">
       <c r="A35" s="18" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -3554,27 +3554,27 @@
       <c r="U35" s="19"/>
       <c r="V35" s="20"/>
       <c r="W35" s="19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="X35" s="19"/>
       <c r="Y35" s="19"/>
       <c r="Z35" s="19"/>
       <c r="AA35" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AB35" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AC35" s="20"/>
       <c r="AD35" s="20"/>
       <c r="AE35" s="20"/>
       <c r="AF35" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="14.65">
       <c r="A36" s="18" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>21</v>
@@ -3618,35 +3618,35 @@
         <v>16</v>
       </c>
       <c r="W36" s="19" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="X36" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Y36" s="19" t="s">
         <v>20</v>
       </c>
       <c r="Z36" s="19"/>
       <c r="AA36" s="20" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="AB36" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AC36" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AD36" s="20" t="s">
         <v>16</v>
       </c>
       <c r="AE36" s="20"/>
       <c r="AF36" s="20" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="14.65">
       <c r="A37" s="18" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>15</v>
@@ -3686,7 +3686,7 @@
         <v>15</v>
       </c>
       <c r="W37" s="19" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="X37" s="19" t="s">
         <v>31</v>
@@ -3694,10 +3694,10 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
       <c r="AA37" s="20" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="AB37" s="20" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="AC37" s="20" t="s">
         <v>31</v>
@@ -3705,12 +3705,12 @@
       <c r="AD37" s="20"/>
       <c r="AE37" s="20"/>
       <c r="AF37" s="20" t="s">
-        <v>161</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="14.65">
       <c r="A38" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>20</v>
@@ -3763,12 +3763,12 @@
       <c r="AD38" s="20"/>
       <c r="AE38" s="20"/>
       <c r="AF38" s="20" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="14.65">
       <c r="A39" s="18" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -3796,7 +3796,7 @@
       <c r="U39" s="19"/>
       <c r="V39" s="20"/>
       <c r="W39" s="19" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="X39" s="19" t="s">
         <v>15</v>
@@ -3809,7 +3809,7 @@
         <v>50</v>
       </c>
       <c r="AB39" s="20" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="AC39" s="20" t="s">
         <v>15</v>
@@ -3819,12 +3819,12 @@
       </c>
       <c r="AE39" s="20"/>
       <c r="AF39" s="20" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="14.65">
       <c r="A40" s="18" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>21</v>
@@ -3844,12 +3844,12 @@
         <v>18</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
       <c r="N40" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O40" s="19" t="s">
         <v>16</v>
@@ -3872,7 +3872,7 @@
         <v>46</v>
       </c>
       <c r="W40" s="19" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="X40" s="19" t="s">
         <v>97</v>
@@ -3882,25 +3882,25 @@
       </c>
       <c r="Z40" s="19"/>
       <c r="AA40" s="20" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="AB40" s="20" t="s">
-        <v>167</v>
+        <v>87</v>
       </c>
       <c r="AC40" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD40" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE40" s="20"/>
       <c r="AF40" s="20" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="14.65">
       <c r="A41" s="18" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>18</v>
@@ -3913,13 +3913,13 @@
         <v>40</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
       <c r="J41" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K41" s="19" t="s">
         <v>46</v>
@@ -3934,7 +3934,7 @@
         <v>35</v>
       </c>
       <c r="O41" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P41" s="19" t="s">
         <v>15</v>
@@ -3956,7 +3956,7 @@
         <v>47</v>
       </c>
       <c r="W41" s="19" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="X41" s="19" t="s">
         <v>98</v>
@@ -3966,25 +3966,25 @@
       </c>
       <c r="Z41" s="19"/>
       <c r="AA41" s="20" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="AB41" s="20" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="AC41" s="20" t="s">
-        <v>173</v>
+        <v>92</v>
       </c>
       <c r="AD41" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE41" s="20"/>
       <c r="AF41" s="20" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="14.65">
       <c r="A42" s="18" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>21</v>
@@ -4036,35 +4036,35 @@
         <v>17</v>
       </c>
       <c r="W42" s="19" t="s">
-        <v>53</v>
+        <v>180</v>
       </c>
       <c r="X42" s="19" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="Y42" s="19" t="s">
         <v>20</v>
       </c>
       <c r="Z42" s="19"/>
       <c r="AA42" s="20" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="AB42" s="20" t="s">
         <v>34</v>
       </c>
       <c r="AC42" s="20" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="AD42" s="20" t="s">
         <v>20</v>
       </c>
       <c r="AE42" s="20"/>
       <c r="AF42" s="20" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="14.65">
       <c r="A43" s="18" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
@@ -4100,7 +4100,7 @@
         <v>20</v>
       </c>
       <c r="W43" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="X43" s="19" t="s">
         <v>15</v>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="Z43" s="19"/>
       <c r="AA43" s="20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AB43" s="20" t="s">
         <v>31</v>
@@ -4123,12 +4123,12 @@
       </c>
       <c r="AE43" s="20"/>
       <c r="AF43" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:32" ht="14.65">
       <c r="A44" s="18" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
@@ -4152,7 +4152,7 @@
       <c r="U44" s="19"/>
       <c r="V44" s="20"/>
       <c r="W44" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X44" s="19" t="s">
         <v>20</v>
@@ -4160,10 +4160,10 @@
       <c r="Y44" s="19"/>
       <c r="Z44" s="19"/>
       <c r="AA44" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AB44" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC44" s="20" t="s">
         <v>20</v>
@@ -4171,12 +4171,12 @@
       <c r="AD44" s="20"/>
       <c r="AE44" s="20"/>
       <c r="AF44" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:32" ht="14.65">
       <c r="A45" s="18" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
@@ -4206,7 +4206,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="20"/>
       <c r="W45" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X45" s="19" t="s">
         <v>40</v>
@@ -4225,29 +4225,29 @@
       <c r="AD45" s="20"/>
       <c r="AE45" s="20"/>
       <c r="AF45" s="20" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="14.65">
       <c r="A46" s="18" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G46" s="19"/>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
       <c r="J46" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K46" s="19" t="s">
         <v>21</v>
@@ -4280,38 +4280,38 @@
         <v>17</v>
       </c>
       <c r="W46" s="19" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="X46" s="19" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="Y46" s="19" t="s">
         <v>40</v>
       </c>
       <c r="Z46" s="19"/>
       <c r="AA46" s="20" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="AB46" s="20" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AC46" s="20" t="s">
-        <v>22</v>
+        <v>189</v>
       </c>
       <c r="AD46" s="20" t="s">
         <v>40</v>
       </c>
       <c r="AE46" s="20"/>
       <c r="AF46" s="20" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="14.65">
       <c r="A47" s="18" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>15</v>
@@ -4358,10 +4358,10 @@
         <v>18</v>
       </c>
       <c r="W47" s="19" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="X47" s="19" t="s">
-        <v>98</v>
+        <v>193</v>
       </c>
       <c r="Y47" s="19" t="s">
         <v>17</v>
@@ -4370,13 +4370,13 @@
         <v>15</v>
       </c>
       <c r="AA47" s="20" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="AB47" s="20" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AC47" s="20" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AD47" s="20" t="s">
         <v>18</v>
@@ -4385,12 +4385,12 @@
         <v>15</v>
       </c>
       <c r="AF47" s="20" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="14.65">
       <c r="A48" s="18" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>18</v>
@@ -4434,7 +4434,7 @@
         <v>17</v>
       </c>
       <c r="W48" s="19" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="X48" s="19" t="s">
         <v>41</v>
@@ -4444,10 +4444,10 @@
       </c>
       <c r="Z48" s="19"/>
       <c r="AA48" s="20" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="AB48" s="20" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AC48" s="20" t="s">
         <v>41</v>
@@ -4457,12 +4457,12 @@
       </c>
       <c r="AE48" s="20"/>
       <c r="AF48" s="20" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:32" ht="14.65">
       <c r="A49" s="18" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>20</v>
@@ -4502,7 +4502,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="20"/>
       <c r="W49" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="X49" s="19" t="s">
         <v>17</v>
@@ -4510,7 +4510,7 @@
       <c r="Y49" s="19"/>
       <c r="Z49" s="19"/>
       <c r="AA49" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB49" s="20" t="s">
         <v>31</v>
@@ -4521,12 +4521,12 @@
       <c r="AD49" s="20"/>
       <c r="AE49" s="20"/>
       <c r="AF49" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:32" ht="14.65">
       <c r="A50" s="18" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>20</v>
@@ -4566,7 +4566,7 @@
         <v>16</v>
       </c>
       <c r="W50" s="19" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
       <c r="X50" s="19" t="s">
         <v>16</v>
@@ -4574,10 +4574,10 @@
       <c r="Y50" s="19"/>
       <c r="Z50" s="19"/>
       <c r="AA50" s="20" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="AB50" s="20" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="AC50" s="20" t="s">
         <v>16</v>
@@ -4585,12 +4585,12 @@
       <c r="AD50" s="20"/>
       <c r="AE50" s="20"/>
       <c r="AF50" s="20" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="14.65">
       <c r="A51" s="18" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>21</v>
@@ -4632,20 +4632,20 @@
         <v>21</v>
       </c>
       <c r="W51" s="19" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="X51" s="19" t="s">
         <v>50</v>
       </c>
       <c r="Y51" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z51" s="19"/>
       <c r="AA51" s="20" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="AB51" s="20" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="AC51" s="20" t="s">
         <v>50</v>
@@ -4655,12 +4655,12 @@
       </c>
       <c r="AE51" s="20"/>
       <c r="AF51" s="20" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="14.65">
       <c r="A52" s="18" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>15</v>
@@ -4700,7 +4700,7 @@
         <v>15</v>
       </c>
       <c r="W52" s="19" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="X52" s="19" t="s">
         <v>18</v>
@@ -4711,7 +4711,7 @@
         <v>26</v>
       </c>
       <c r="AB52" s="20" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="AC52" s="20" t="s">
         <v>18</v>
@@ -4719,22 +4719,22 @@
       <c r="AD52" s="20"/>
       <c r="AE52" s="20"/>
       <c r="AF52" s="20" t="s">
-        <v>22</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:32" ht="14.65">
       <c r="A53" s="18" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F53" s="19" t="s">
         <v>35</v>
@@ -4745,19 +4745,19 @@
       <c r="H53" s="19"/>
       <c r="I53" s="19"/>
       <c r="J53" s="20" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="K53" s="19" t="s">
         <v>35</v>
       </c>
       <c r="L53" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="M53" s="19" t="s">
         <v>20</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O53" s="19" t="s">
         <v>35</v>
@@ -4781,38 +4781,38 @@
         <v>15</v>
       </c>
       <c r="V53" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="W53" s="19" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="X53" s="19" t="s">
-        <v>209</v>
+        <v>131</v>
       </c>
       <c r="Y53" s="19" t="s">
         <v>26</v>
       </c>
       <c r="Z53" s="19"/>
       <c r="AA53" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="AB53" s="20" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="AC53" s="20" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="AD53" s="20" t="s">
-        <v>22</v>
+        <v>189</v>
       </c>
       <c r="AE53" s="20"/>
       <c r="AF53" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:32" ht="14.65">
       <c r="A54" s="18" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>17</v>
@@ -4862,7 +4862,7 @@
         <v>17</v>
       </c>
       <c r="W54" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="X54" s="19" t="s">
         <v>35</v>
@@ -4872,25 +4872,25 @@
       </c>
       <c r="Z54" s="19"/>
       <c r="AA54" s="20" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AB54" s="20" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="AC54" s="20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AD54" s="20" t="s">
         <v>17</v>
       </c>
       <c r="AE54" s="20"/>
       <c r="AF54" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:32" ht="14.65">
       <c r="A55" s="18" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>99</v>
@@ -4902,10 +4902,10 @@
         <v>15</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G55" s="19" t="s">
         <v>20</v>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="I55" s="19"/>
       <c r="J55" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K55" s="19" t="s">
         <v>29</v>
@@ -4933,59 +4933,59 @@
       </c>
       <c r="Q55" s="19"/>
       <c r="R55" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="S55" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="T55" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U55" s="19"/>
       <c r="V55" s="20" t="s">
         <v>32</v>
       </c>
       <c r="W55" s="19" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="X55" s="19" t="s">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="Y55" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z55" s="19"/>
       <c r="AA55" s="20" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AB55" s="20" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="AC55" s="20" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="AD55" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AE55" s="20"/>
       <c r="AF55" s="20" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:32" ht="14.65">
       <c r="A56" s="18" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G56" s="19" t="s">
         <v>15</v>
@@ -4996,7 +4996,7 @@
         <v>42</v>
       </c>
       <c r="K56" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L56" s="19"/>
       <c r="M56" s="19" t="s">
@@ -5021,38 +5021,38 @@
         <v>15</v>
       </c>
       <c r="V56" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W56" s="19" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="X56" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Y56" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Z56" s="19"/>
       <c r="AA56" s="20" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="AB56" s="20" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="AC56" s="20" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="AD56" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE56" s="20"/>
       <c r="AF56" s="20" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:32" ht="14.65">
       <c r="A57" s="18" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B57" s="19" t="s">
         <v>47</v>
@@ -5073,10 +5073,10 @@
         <v>15</v>
       </c>
       <c r="J57" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K57" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L57" s="19" t="s">
         <v>20</v>
@@ -5093,63 +5093,63 @@
       </c>
       <c r="Q57" s="19"/>
       <c r="R57" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S57" s="19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="T57" s="19"/>
       <c r="U57" s="19" t="s">
         <v>15</v>
       </c>
       <c r="V57" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W57" s="19" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="X57" s="19" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="Y57" s="19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="Z57" s="19"/>
       <c r="AA57" s="20" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="AB57" s="20" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="AC57" s="20" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="AD57" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AE57" s="20" t="s">
         <v>15</v>
       </c>
       <c r="AF57" s="20" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:32" ht="14.65">
       <c r="A58" s="18" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G58" s="19" t="s">
         <v>19</v>
@@ -5172,7 +5172,7 @@
         <v>46</v>
       </c>
       <c r="O58" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P58" s="19" t="s">
         <v>21</v>
@@ -5192,35 +5192,35 @@
         <v>43</v>
       </c>
       <c r="W58" s="19" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="X58" s="19" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="Y58" s="19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="Z58" s="19"/>
       <c r="AA58" s="20" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="AB58" s="20" t="s">
-        <v>239</v>
+        <v>63</v>
       </c>
       <c r="AC58" s="20" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="AD58" s="20" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="AE58" s="20"/>
       <c r="AF58" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:32" ht="14.65">
       <c r="A59" s="18" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B59" s="19" t="s">
         <v>20</v>
@@ -5259,14 +5259,14 @@
       </c>
       <c r="Q59" s="19"/>
       <c r="R59" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S59" s="19"/>
       <c r="T59" s="19"/>
       <c r="U59" s="19"/>
       <c r="V59" s="20"/>
       <c r="W59" s="19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="X59" s="19" t="s">
         <v>46</v>
@@ -5274,10 +5274,10 @@
       <c r="Y59" s="19"/>
       <c r="Z59" s="19"/>
       <c r="AA59" s="20" t="s">
-        <v>22</v>
+        <v>193</v>
       </c>
       <c r="AB59" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AC59" s="20" t="s">
         <v>35</v>
@@ -5287,12 +5287,12 @@
       </c>
       <c r="AE59" s="20"/>
       <c r="AF59" s="20" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:32" ht="14.65">
       <c r="A60" s="18" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B60" s="19" t="s">
         <v>18</v>
@@ -5336,7 +5336,7 @@
         <v>18</v>
       </c>
       <c r="W60" s="19" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="X60" s="19" t="s">
         <v>40</v>
@@ -5346,10 +5346,10 @@
       </c>
       <c r="Z60" s="19"/>
       <c r="AA60" s="20" t="s">
-        <v>105</v>
+        <v>247</v>
       </c>
       <c r="AB60" s="20" t="s">
-        <v>83</v>
+        <v>248</v>
       </c>
       <c r="AC60" s="20" t="s">
         <v>40</v>
@@ -5359,12 +5359,12 @@
       </c>
       <c r="AE60" s="20"/>
       <c r="AF60" s="20" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:32" ht="14.65">
       <c r="A61" s="18" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>15</v>
@@ -5377,13 +5377,13 @@
         <v>20</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
       <c r="J61" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K61" s="19" t="s">
         <v>17</v>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="Q61" s="19"/>
       <c r="R61" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S61" s="19" t="s">
         <v>19</v>
@@ -5416,39 +5416,39 @@
         <v>18</v>
       </c>
       <c r="W61" s="19" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="X61" s="19" t="s">
-        <v>248</v>
+        <v>53</v>
       </c>
       <c r="Y61" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Z61" s="19" t="s">
         <v>15</v>
       </c>
       <c r="AA61" s="20" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="AB61" s="20" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="AC61" s="20" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="AD61" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AE61" s="20" t="s">
         <v>15</v>
       </c>
       <c r="AF61" s="20" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:32" ht="14.65">
       <c r="A62" s="18" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>16</v>
@@ -5492,46 +5492,46 @@
         <v>16</v>
       </c>
       <c r="W62" s="19" t="s">
-        <v>253</v>
+        <v>68</v>
       </c>
       <c r="X62" s="19" t="s">
         <v>21</v>
       </c>
       <c r="Y62" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Z62" s="19"/>
       <c r="AA62" s="20" t="s">
-        <v>24</v>
+        <v>239</v>
       </c>
       <c r="AB62" s="20" t="s">
-        <v>254</v>
+        <v>129</v>
       </c>
       <c r="AC62" s="20" t="s">
         <v>21</v>
       </c>
       <c r="AD62" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AE62" s="20"/>
       <c r="AF62" s="20" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="63" spans="1:32" ht="14.65">
       <c r="A63" s="18" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
       <c r="E63" s="20" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G63" s="19" t="s">
         <v>15</v>
@@ -5539,7 +5539,7 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
       <c r="J63" s="20" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="K63" s="19" t="s">
         <v>45</v>
@@ -5560,25 +5560,25 @@
         <v>18</v>
       </c>
       <c r="S63" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="T63" s="19"/>
       <c r="U63" s="19"/>
       <c r="V63" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="W63" s="19" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="X63" s="19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Y63" s="19" t="s">
         <v>21</v>
       </c>
       <c r="Z63" s="19"/>
       <c r="AA63" s="20" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AB63" s="20" t="s">
         <v>259</v>
@@ -5591,20 +5591,20 @@
       </c>
       <c r="AE63" s="20"/>
       <c r="AF63" s="20" t="s">
-        <v>260</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:32" ht="14.65">
       <c r="A64" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
       <c r="E64" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>21</v>
@@ -5620,22 +5620,22 @@
         <v>40</v>
       </c>
       <c r="K64" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L64" s="19" t="s">
         <v>15</v>
       </c>
       <c r="M64" s="19"/>
       <c r="N64" s="20" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="O64" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P64" s="19"/>
       <c r="Q64" s="19"/>
       <c r="R64" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S64" s="19" t="s">
         <v>21</v>
@@ -5646,35 +5646,35 @@
         <v>21</v>
       </c>
       <c r="W64" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X64" s="19" t="s">
-        <v>263</v>
+        <v>97</v>
       </c>
       <c r="Y64" s="19" t="s">
         <v>17</v>
       </c>
       <c r="Z64" s="19"/>
       <c r="AA64" s="20" t="s">
-        <v>264</v>
+        <v>87</v>
       </c>
       <c r="AB64" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AC64" s="20" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="AD64" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AE64" s="20"/>
       <c r="AF64" s="20" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:32" ht="14.65">
       <c r="A65" s="18" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>21</v>
@@ -5720,7 +5720,7 @@
         <v>19</v>
       </c>
       <c r="W65" s="19" t="s">
-        <v>268</v>
+        <v>93</v>
       </c>
       <c r="X65" s="19" t="s">
         <v>17</v>
@@ -5730,25 +5730,25 @@
       </c>
       <c r="Z65" s="19"/>
       <c r="AA65" s="20" t="s">
-        <v>105</v>
+        <v>247</v>
       </c>
       <c r="AB65" s="20" t="s">
-        <v>83</v>
+        <v>248</v>
       </c>
       <c r="AC65" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AD65" s="20" t="s">
         <v>16</v>
       </c>
       <c r="AE65" s="20"/>
       <c r="AF65" s="20" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:32" ht="14.65">
       <c r="A66" s="18" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>15</v>
@@ -5788,7 +5788,7 @@
         <v>21</v>
       </c>
       <c r="W66" s="19" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
       <c r="X66" s="19" t="s">
         <v>18</v>
@@ -5798,10 +5798,10 @@
       </c>
       <c r="Z66" s="19"/>
       <c r="AA66" s="20" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AB66" s="20" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="AC66" s="20" t="s">
         <v>18</v>
@@ -5811,12 +5811,12 @@
       </c>
       <c r="AE66" s="20"/>
       <c r="AF66" s="20" t="s">
-        <v>161</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:32" ht="14.65">
       <c r="A67" s="18" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
@@ -5840,7 +5840,7 @@
       <c r="U67" s="19"/>
       <c r="V67" s="20"/>
       <c r="W67" s="19" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="X67" s="19" t="s">
         <v>16</v>
@@ -5848,10 +5848,10 @@
       <c r="Y67" s="19"/>
       <c r="Z67" s="19"/>
       <c r="AA67" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB67" s="20" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="AC67" s="20" t="s">
         <v>16</v>
@@ -5859,12 +5859,12 @@
       <c r="AD67" s="20"/>
       <c r="AE67" s="20"/>
       <c r="AF67" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:32" ht="14.65">
       <c r="A68" s="18" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
@@ -5908,20 +5908,20 @@
         <v>16</v>
       </c>
       <c r="W68" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="X68" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Y68" s="19" t="s">
         <v>20</v>
       </c>
       <c r="Z68" s="19"/>
       <c r="AA68" s="20" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="AB68" s="20" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="AC68" s="20" t="s">
         <v>45</v>
@@ -5931,15 +5931,15 @@
       </c>
       <c r="AE68" s="20"/>
       <c r="AF68" s="20" t="s">
-        <v>25</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:32" ht="14.65">
       <c r="A69" s="18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C69" s="19" t="s">
         <v>20</v>
@@ -5968,14 +5968,14 @@
         <v>43</v>
       </c>
       <c r="O69" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P69" s="19" t="s">
         <v>15</v>
       </c>
       <c r="Q69" s="19"/>
       <c r="R69" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="S69" s="19" t="s">
         <v>42</v>
@@ -5986,20 +5986,20 @@
         <v>42</v>
       </c>
       <c r="W69" s="19" t="s">
-        <v>183</v>
+        <v>272</v>
       </c>
       <c r="X69" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="Y69" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Z69" s="19"/>
       <c r="AA69" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AB69" s="20" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AC69" s="20" t="s">
         <v>49</v>
@@ -6009,12 +6009,12 @@
       </c>
       <c r="AE69" s="20"/>
       <c r="AF69" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:32" ht="14.65">
       <c r="A70" s="18" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B70" s="19"/>
       <c r="C70" s="19"/>
@@ -6050,7 +6050,7 @@
         <v>15</v>
       </c>
       <c r="W70" s="19" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="X70" s="19" t="s">
         <v>16</v>
@@ -6058,10 +6058,10 @@
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
       <c r="AA70" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AB70" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AC70" s="20" t="s">
         <v>21</v>
@@ -6069,12 +6069,12 @@
       <c r="AD70" s="20"/>
       <c r="AE70" s="20"/>
       <c r="AF70" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:32" ht="14.65">
       <c r="A71" s="18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
@@ -6106,7 +6106,7 @@
       <c r="U71" s="19"/>
       <c r="V71" s="20"/>
       <c r="W71" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="X71" s="19" t="s">
         <v>15</v>
@@ -6116,10 +6116,10 @@
       </c>
       <c r="Z71" s="19"/>
       <c r="AA71" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AB71" s="20" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="AC71" s="20" t="s">
         <v>15</v>
@@ -6129,12 +6129,12 @@
       </c>
       <c r="AE71" s="20"/>
       <c r="AF71" s="20" t="s">
-        <v>263</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="14.65">
       <c r="A72" s="18" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
@@ -6165,23 +6165,23 @@
         <v>42</v>
       </c>
       <c r="X72" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y72" s="19"/>
       <c r="Z72" s="19"/>
       <c r="AA72" s="20" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="AB72" s="20" t="s">
         <v>45</v>
       </c>
       <c r="AC72" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AD72" s="20"/>
       <c r="AE72" s="20"/>
       <c r="AF72" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:32" ht="14.65">
@@ -6233,7 +6233,7 @@
         <v>40</v>
       </c>
       <c r="AB73" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC73" s="20" t="s">
         <v>15</v>
@@ -6245,7 +6245,7 @@
         <v>15</v>
       </c>
       <c r="AF73" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:32" ht="14.65">
@@ -6253,22 +6253,22 @@
         <v>8</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>41</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H74" s="20" t="s">
         <v>41</v>
@@ -6277,52 +6277,52 @@
         <v>15</v>
       </c>
       <c r="J74" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="K74" s="20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L74" s="20" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="M74" s="20" t="s">
         <v>18</v>
       </c>
       <c r="N74" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O74" s="20" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="P74" s="20" t="s">
-        <v>199</v>
+        <v>266</v>
       </c>
       <c r="Q74" s="20" t="s">
         <v>18</v>
       </c>
       <c r="R74" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="S74" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="S74" s="20" t="s">
+      <c r="T74" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="U74" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="V74" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="T74" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="U74" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="V74" s="20" t="s">
+      <c r="W74" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="W74" s="20" t="s">
+      <c r="X74" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="X74" s="20" t="s">
+      <c r="Y74" s="20" t="s">
         <v>292</v>
-      </c>
-      <c r="Y74" s="20" t="s">
-        <v>288</v>
       </c>
       <c r="Z74" s="20" t="s">
         <v>41</v>
@@ -6340,7 +6340,7 @@
         <v>296</v>
       </c>
       <c r="AE74" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF74" s="20" t="s">
         <v>297</v>

</xml_diff>